<commit_message>
Actualización de comerciales en el Excel
</commit_message>
<xml_diff>
--- a/data/PROYECTO_APP_CLIENTES.xlsx
+++ b/data/PROYECTO_APP_CLIENTES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gigante/Desktop/Proyecto Visualizacion 2025/pedidos_comerciales/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCFE281-8C3E-814D-A2B8-4861CF362AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D095AA-284F-9C44-983B-BBBA64D79568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9254" uniqueCount="3037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9257" uniqueCount="3040">
   <si>
     <t>Suplemento Hoja Piso Corrido E-150 Anod. Plata L=6,5m</t>
   </si>
@@ -13608,6 +13608,15 @@
   </si>
   <si>
     <t>articulos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGNACIO </t>
+  </si>
+  <si>
+    <t>ANDRES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JORDI MARINA </t>
   </si>
 </sst>
 </file>
@@ -14413,8 +14422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED71349-4D8D-4590-81BA-63A1C11AD5DA}">
   <dimension ref="A1:B664"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+    <sheetView topLeftCell="A660" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -50815,7 +50824,7 @@
   <dimension ref="A1:C442"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -50859,14 +50868,20 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="57"/>
+      <c r="A8" s="57" t="s">
+        <v>3037</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="57"/>
+      <c r="A9" s="57" t="s">
+        <v>3038</v>
+      </c>
       <c r="C9" s="60"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="57"/>
+      <c r="A10" s="57" t="s">
+        <v>3039</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="57"/>

</xml_diff>